<commit_message>
Update EV charger costs based on NAP study
</commit_message>
<xml_diff>
--- a/InputData/trans/EVCC/EV Charger Cost.xlsx
+++ b/InputData/trans/EVCC/EV Charger Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\trans\EVCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\trans\EVCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D956A065-A3EB-4C93-8419-E8791BDAC14C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBB0232-F92E-4504-A060-6868C576819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>https://afdc.energy.gov/files/u/publication/evse_cost_report_2015.pdf</t>
-  </si>
-  <si>
-    <t>Costs Associated With Non-Residential Electric Vehicle Supply Equipment</t>
-  </si>
-  <si>
     <t>U.S. Department of Energy</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>EVSE Type</t>
   </si>
   <si>
-    <t>Level 1</t>
-  </si>
-  <si>
     <t>Level 2</t>
   </si>
   <si>
@@ -79,27 +70,15 @@
     <t>Currency Conversion</t>
   </si>
   <si>
-    <t>We assume the costs given in this Nov 2015 document</t>
-  </si>
-  <si>
-    <t>are in 2015 dollars.  We convert to 2012 dollars via:</t>
-  </si>
-  <si>
     <t>EVCC Electric Vehicle Charger Cost</t>
   </si>
   <si>
-    <t>Page 11, Table 1 and Page 17, Table 2</t>
-  </si>
-  <si>
     <t>Capital Costs</t>
   </si>
   <si>
     <t>Avg. installation cost</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Installation Costs</t>
   </si>
   <si>
@@ -146,6 +125,42 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Level 2 commercial</t>
+  </si>
+  <si>
+    <t>The National Academies Press</t>
+  </si>
+  <si>
+    <t>Assessment of Technologies for Improving Light-Duty Vehicle Fuel Economy 2025-2035</t>
+  </si>
+  <si>
+    <t>https://www.nap.edu/download/26092#</t>
+  </si>
+  <si>
+    <t>Tables 5.13, 5.14, and 5.15</t>
+  </si>
+  <si>
+    <t>We assume the costs given in this document</t>
+  </si>
+  <si>
+    <t>are in 2020 dollars.  We convert to 2012 dollars via:</t>
+  </si>
+  <si>
+    <t>To determine the costs for Fast DC and Level 2 capital and installation costs, we take</t>
+  </si>
+  <si>
+    <t xml:space="preserve">representative costs from the table (e.g. choosing </t>
+  </si>
+  <si>
+    <t>Average DCFC</t>
+  </si>
+  <si>
+    <t>Average Level 2</t>
+  </si>
+  <si>
+    <t>Average DCFC (150 kW taken as representative)</t>
   </si>
 </sst>
 </file>
@@ -153,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -228,7 +243,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -246,6 +261,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>11628</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>148795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDFF8F3D-26E4-4C44-A635-4589725B387A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4108450" y="139701"/>
+          <a:ext cx="7650678" cy="3323794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>443407</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>126760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3137AFEA-E9F6-46CD-BF9A-726F85A6030C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4057650" y="3543300"/>
+          <a:ext cx="8742857" cy="1923810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>567371</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>135990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B84F1A4-2676-4D48-8FFD-BD0DFCC3A035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="5619750"/>
+          <a:ext cx="7628571" cy="4276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,323 +663,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="67.5703125" customWidth="1"/>
+    <col min="2" max="2" width="67.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0.9686815713640794</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.88711067149387013</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{0C92D522-9338-48F9-BF08-9A9FE950F9B8}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{0C92D522-9338-48F9-BF08-9A9FE950F9B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>2500</v>
       </c>
       <c r="C3">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>10000</v>
-      </c>
-      <c r="C5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="5">
+        <f>AVERAGE(20000,75600,128000)</f>
+        <v>74533.333333333328</v>
+      </c>
+      <c r="C4" s="5">
+        <f>AVERAGE(35800,100000,150000)</f>
+        <v>95266.666666666672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5">
+        <f>AVERAGE(4148,3039,2745,2837)</f>
+        <v>3192.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="5">
+        <f>AVERAGE(47781,38047,28312,18577)</f>
+        <v>33179.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>57940</v>
+      </c>
+      <c r="C13" s="8">
+        <f>B13/SUM(B13:B14)</f>
+        <v>0.84215116279069768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>10860</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B14/SUM(B13:B14)</f>
+        <v>0.15784883720930232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B17" s="5">
+        <f>AVERAGE(B3:C3)*C13+AVERAGE(B4:C4)*C14</f>
+        <v>16517.325581395347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>57940</v>
-      </c>
-      <c r="C16" s="8">
-        <f>B16/SUM(B16:B17)</f>
-        <v>0.84215116279069768</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>10860</v>
-      </c>
-      <c r="C17" s="8">
-        <f>B17/SUM(B16:B17)</f>
-        <v>0.15784883720930232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="5">
-        <f>AVERAGE(B4:C4)*C16+AVERAGE(B5:C5)*C17</f>
-        <v>6851.6424418604647</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="5">
-        <f>B10*C16+B11*C17</f>
-        <v>5841.2790697674418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="5">
-        <f>SUM(B20:B21)</f>
-        <v>12692.921511627907</v>
+      <c r="B18" s="5">
+        <f>B8*C13+B9*C14</f>
+        <v>7925.6630813953489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5">
+        <f>SUM(B17:B18)</f>
+        <v>24442.988662790696</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -838,26 +981,28 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5">
-        <f>Data!B22</f>
-        <v>12692.921511627907</v>
+        <f>Data!B19</f>
+        <v>24442.988662790696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>